<commit_message>
todo listo antes de la presentacion
</commit_message>
<xml_diff>
--- a/excel_reports/averageDistancesTraveled.xlsx
+++ b/excel_reports/averageDistancesTraveled.xlsx
@@ -2,28 +2,29 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr hidePivotFieldList="1"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\OneDrive\Escritorio\repos\resumenipa\excel_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9190BDCA-B576-4B50-946F-D6196B48697E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F06530-D2C3-4B9A-94CB-CC8C428190A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId2"/>
+    <pivotCache cacheId="7" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
   <si>
     <t>total</t>
   </si>
@@ -84,6 +85,12 @@
   <si>
     <t>Promedio de la mascota (Kilometros)</t>
   </si>
+  <si>
+    <t>Sum of Promedio KM</t>
+  </si>
+  <si>
+    <t>Sum of Total KM's</t>
+  </si>
 </sst>
 </file>
 
@@ -101,6 +108,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,7 +151,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -416,7 +424,17 @@
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.6495521393159191E-2"/>
+          <c:y val="5.5555555555555552E-2"/>
+          <c:w val="0.63413906595008962"/>
+          <c:h val="0.73143518518518513"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -855,7 +873,839 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[averageDistancesTraveled.xlsx]Sheet2!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-EC"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$2:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Amigo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chimu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lara</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maddy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mora</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Neutron</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>René</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Sambayón</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sari</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tiana</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.0939999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2175000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7875000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7225000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5857142857142861</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.7050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6437499999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.574</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9A91-43D7-AC10-706F0F6F0E71}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1595322912"/>
+        <c:axId val="2091934656"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1595322912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2091934656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2091934656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1595322912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-EC"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[averageDistancesTraveled.xlsx]Sheet2!PivotTable2</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-EC"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$22:$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Amigo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chimu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lara</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maddy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mora</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Neutron</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>René</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Sambayón</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sari</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tiana</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$22:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>25.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.82</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA7F-49C2-B9A2-2F3FD80FE629}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1595320512"/>
+        <c:axId val="2091930192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1595320512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2091930192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2091930192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1595320512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-EC"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1398,6 +2248,1012 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1431,6 +3287,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF5DC743-B68E-6929-7C07-809B98EE9529}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64C82B9-FE2D-DED9-D5EC-394BDCF96F27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1530,7 +3463,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E5FC148F-4D2A-4CE8-BD0F-E6B43BC62ED4}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E5FC148F-4D2A-4CE8-BD0F-E6B43BC62ED4}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="J1:L12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -1672,6 +3605,202 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6FAD6594-693C-4FE6-8317-D2893A924AB1}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A21:B32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item x="7"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total KM's" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3CBA6441-F673-4791-B561-5C6E40FA9CEF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A1:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item x="7"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Promedio KM" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1959,8 +4088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,10 +4154,10 @@
       <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2">
         <v>25.47</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2">
         <v>5.0939999999999994</v>
       </c>
     </row>
@@ -2057,10 +4186,10 @@
       <c r="J3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3">
         <v>20.87</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3">
         <v>5.2175000000000002</v>
       </c>
     </row>
@@ -2089,10 +4218,10 @@
       <c r="J4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4">
         <v>22.3</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4">
         <v>2.7875000000000001</v>
       </c>
     </row>
@@ -2121,10 +4250,10 @@
       <c r="J5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5">
         <v>59.74</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5">
         <v>11.948</v>
       </c>
     </row>
@@ -2153,10 +4282,10 @@
       <c r="J6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6">
         <v>14.89</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6">
         <v>3.7225000000000001</v>
       </c>
     </row>
@@ -2185,10 +4314,10 @@
       <c r="J7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7">
         <v>11.1</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7">
         <v>1.5857142857142861</v>
       </c>
     </row>
@@ -2217,10 +4346,10 @@
       <c r="J8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8">
         <v>14.82</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8">
         <v>3.7050000000000001</v>
       </c>
     </row>
@@ -2249,10 +4378,10 @@
       <c r="J9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9">
         <v>21.15</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9">
         <v>2.6437499999999998</v>
       </c>
     </row>
@@ -2281,10 +4410,10 @@
       <c r="J10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10">
         <v>31.6</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10">
         <v>3.16</v>
       </c>
     </row>
@@ -2313,10 +4442,10 @@
       <c r="J11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11">
         <v>52.87</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11">
         <v>10.574</v>
       </c>
     </row>
@@ -2324,10 +4453,10 @@
       <c r="J12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12">
         <v>274.80999999999995</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12">
         <v>50.437964285714273</v>
       </c>
     </row>
@@ -2335,4 +4464,216 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C3825F-7F2D-445E-BE65-2E8EB8844C10}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5">
+        <v>5.0939999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5.2175000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2.7875000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>11.948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>3.7225000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1.5857142857142861</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3.7050000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2.6437499999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10.574</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5">
+        <v>50.437964285714273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="5">
+        <v>25.47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5">
+        <v>20.87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="5">
+        <v>59.74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="5">
+        <v>14.89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="5">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="5">
+        <v>14.82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="5">
+        <v>21.15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="5">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="5">
+        <v>52.87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="5">
+        <v>274.80999999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>